<commit_message>
update to latest release of monthly eia data
</commit_message>
<xml_diff>
--- a/data/Table_1.2_Primary_Energy_Production_by_Source.xlsx
+++ b/data/Table_1.2_Primary_Energy_Production_by_Source.xlsx
@@ -21,13 +21,13 @@
     <t>U.S. Energy Information Administration</t>
   </si>
   <si>
-    <t>July 2020 Monthly Energy Review</t>
+    <t>August 2020 Monthly Energy Review</t>
   </si>
   <si>
-    <t>Release Date: July 28, 2020</t>
+    <t>Release Date: August 26, 2020</t>
   </si>
   <si>
-    <t>Next Update: August 26, 2020</t>
+    <t>Next Update: September 24, 2020</t>
   </si>
   <si>
     <t>Table 1.2 Primary Energy Production by Source</t>
@@ -488,7 +488,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N580"/>
+  <dimension ref="A1:N581"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A13" sqref="A13"/>
@@ -24928,13 +24928,13 @@
         <v>2.848784</v>
       </c>
       <c r="D565">
-        <v>2.094291</v>
+        <v>2.095812</v>
       </c>
       <c r="E565">
         <v>0.508212</v>
       </c>
       <c r="F565">
-        <v>6.782465</v>
+        <v>6.783986</v>
       </c>
       <c r="G565">
         <v>0.770542</v>
@@ -24958,7 +24958,7 @@
         <v>0.964568</v>
       </c>
       <c r="N565">
-        <v>8.517575</v>
+        <v>8.519096</v>
       </c>
     </row>
     <row r="566" spans="1:14">
@@ -24972,13 +24972,13 @@
         <v>2.59617</v>
       </c>
       <c r="D566">
-        <v>1.861729</v>
+        <v>1.863288</v>
       </c>
       <c r="E566">
         <v>0.475284</v>
       </c>
       <c r="F566">
-        <v>6.111858</v>
+        <v>6.113417</v>
       </c>
       <c r="G566">
         <v>0.676594</v>
@@ -25002,7 +25002,7 @@
         <v>0.884766</v>
       </c>
       <c r="N566">
-        <v>7.673218</v>
+        <v>7.674777</v>
       </c>
     </row>
     <row r="567" spans="1:14">
@@ -25016,13 +25016,13 @@
         <v>2.89091</v>
       </c>
       <c r="D567">
-        <v>2.100533</v>
+        <v>2.108582</v>
       </c>
       <c r="E567">
         <v>0.528689</v>
       </c>
       <c r="F567">
-        <v>6.646332</v>
+        <v>6.65438</v>
       </c>
       <c r="G567">
         <v>0.680408</v>
@@ -25046,7 +25046,7 @@
         <v>1.003725</v>
       </c>
       <c r="N567">
-        <v>8.330465</v>
+        <v>8.338513</v>
       </c>
     </row>
     <row r="568" spans="1:14">
@@ -25060,13 +25060,13 @@
         <v>2.812496</v>
       </c>
       <c r="D568">
-        <v>2.072258</v>
+        <v>2.074305</v>
       </c>
       <c r="E568">
         <v>0.517954</v>
       </c>
       <c r="F568">
-        <v>6.635801</v>
+        <v>6.637848</v>
       </c>
       <c r="G568">
         <v>0.633374</v>
@@ -25090,7 +25090,7 @@
         <v>1.039877</v>
       </c>
       <c r="N568">
-        <v>8.309052</v>
+        <v>8.311099</v>
       </c>
     </row>
     <row r="569" spans="1:14">
@@ -25104,13 +25104,13 @@
         <v>2.8907</v>
       </c>
       <c r="D569">
-        <v>2.13964</v>
+        <v>2.148482</v>
       </c>
       <c r="E569">
         <v>0.54096</v>
       </c>
       <c r="F569">
-        <v>6.81811</v>
+        <v>6.826952</v>
       </c>
       <c r="G569">
         <v>0.701777</v>
@@ -25134,7 +25134,7 @@
         <v>1.070751</v>
       </c>
       <c r="N569">
-        <v>8.590637</v>
+        <v>8.59948</v>
       </c>
     </row>
     <row r="570" spans="1:14">
@@ -25148,13 +25148,13 @@
         <v>2.837185</v>
       </c>
       <c r="D570">
-        <v>2.061565</v>
+        <v>2.066245</v>
       </c>
       <c r="E570">
         <v>0.518607</v>
       </c>
       <c r="F570">
-        <v>6.561406</v>
+        <v>6.566086</v>
       </c>
       <c r="G570">
         <v>0.719355</v>
@@ -25178,7 +25178,7 @@
         <v>1.009359</v>
       </c>
       <c r="N570">
-        <v>8.29012</v>
+        <v>8.2948</v>
       </c>
     </row>
     <row r="571" spans="1:14">
@@ -25192,13 +25192,13 @@
         <v>2.934294</v>
       </c>
       <c r="D571">
-        <v>2.088399</v>
+        <v>2.087701</v>
       </c>
       <c r="E571">
         <v>0.523192</v>
       </c>
       <c r="F571">
-        <v>6.740407</v>
+        <v>6.739709</v>
       </c>
       <c r="G571">
         <v>0.754836</v>
@@ -25222,7 +25222,7 @@
         <v>0.992281</v>
       </c>
       <c r="N571">
-        <v>8.487524</v>
+        <v>8.486826</v>
       </c>
     </row>
     <row r="572" spans="1:14">
@@ -25236,13 +25236,13 @@
         <v>2.999831</v>
       </c>
       <c r="D572">
-        <v>2.187617</v>
+        <v>2.194686</v>
       </c>
       <c r="E572">
         <v>0.528534</v>
       </c>
       <c r="F572">
-        <v>7.005189</v>
+        <v>7.012259</v>
       </c>
       <c r="G572">
         <v>0.751826</v>
@@ -25266,7 +25266,7 @@
         <v>0.94791</v>
       </c>
       <c r="N572">
-        <v>8.704925</v>
+        <v>8.711995</v>
       </c>
     </row>
     <row r="573" spans="1:14">
@@ -25280,13 +25280,13 @@
         <v>2.936442</v>
       </c>
       <c r="D573">
-        <v>2.133079</v>
+        <v>2.135927</v>
       </c>
       <c r="E573">
         <v>0.539813</v>
       </c>
       <c r="F573">
-        <v>6.792619</v>
+        <v>6.795468</v>
       </c>
       <c r="G573">
         <v>0.690695</v>
@@ -25310,7 +25310,7 @@
         <v>0.897109</v>
       </c>
       <c r="N573">
-        <v>8.380423</v>
+        <v>8.383272</v>
       </c>
     </row>
     <row r="574" spans="1:14">
@@ -25324,13 +25324,13 @@
         <v>3.0791</v>
       </c>
       <c r="D574">
-        <v>2.238732</v>
+        <v>2.238454</v>
       </c>
       <c r="E574">
         <v>0.561523</v>
       </c>
       <c r="F574">
-        <v>7.043935</v>
+        <v>7.043658</v>
       </c>
       <c r="G574">
         <v>0.648551</v>
@@ -25354,7 +25354,7 @@
         <v>0.93344</v>
       </c>
       <c r="N574">
-        <v>8.625926</v>
+        <v>8.625649</v>
       </c>
     </row>
     <row r="575" spans="1:14">
@@ -25368,13 +25368,13 @@
         <v>2.994292</v>
       </c>
       <c r="D575">
-        <v>2.199364</v>
+        <v>2.198251</v>
       </c>
       <c r="E575">
         <v>0.538027</v>
       </c>
       <c r="F575">
-        <v>6.831675</v>
+        <v>6.830562</v>
       </c>
       <c r="G575">
         <v>0.670431</v>
@@ -25398,7 +25398,7 @@
         <v>0.924473</v>
       </c>
       <c r="N575">
-        <v>8.426579</v>
+        <v>8.425466</v>
       </c>
     </row>
     <row r="576" spans="1:14">
@@ -25412,13 +25412,13 @@
         <v>3.082153</v>
       </c>
       <c r="D576">
-        <v>2.263269</v>
+        <v>2.261337</v>
       </c>
       <c r="E576">
         <v>0.555813</v>
       </c>
       <c r="F576">
-        <v>6.9777</v>
+        <v>6.975768</v>
       </c>
       <c r="G576">
         <v>0.763984</v>
@@ -25442,7 +25442,7 @@
         <v>0.968717</v>
       </c>
       <c r="N576">
-        <v>8.710401</v>
+        <v>8.708469</v>
       </c>
     </row>
     <row r="577" spans="1:14">
@@ -25456,13 +25456,13 @@
         <v>3.047073</v>
       </c>
       <c r="D577">
-        <v>2.252936</v>
+        <v>2.252986</v>
       </c>
       <c r="E577">
         <v>0.575331</v>
       </c>
       <c r="F577">
-        <v>6.999839</v>
+        <v>6.99989</v>
       </c>
       <c r="G577">
         <v>0.775803</v>
@@ -25486,7 +25486,7 @@
         <v>0.996503</v>
       </c>
       <c r="N577">
-        <v>8.772146</v>
+        <v>8.772196</v>
       </c>
     </row>
     <row r="578" spans="1:14">
@@ -25497,16 +25497,16 @@
         <v>0.958775</v>
       </c>
       <c r="C578">
-        <v>2.84342</v>
+        <v>2.839233</v>
       </c>
       <c r="D578">
-        <v>2.106446</v>
+        <v>2.106109</v>
       </c>
       <c r="E578">
         <v>0.519376</v>
       </c>
       <c r="F578">
-        <v>6.428017</v>
+        <v>6.423493</v>
       </c>
       <c r="G578">
         <v>0.689511</v>
@@ -25530,7 +25530,7 @@
         <v>0.992812</v>
       </c>
       <c r="N578">
-        <v>8.110339</v>
+        <v>8.105815</v>
       </c>
     </row>
     <row r="579" spans="1:14">
@@ -25541,16 +25541,16 @@
         <v>0.930999</v>
       </c>
       <c r="C579">
-        <v>3.026773</v>
+        <v>3.029791</v>
       </c>
       <c r="D579">
-        <v>2.248685</v>
+        <v>2.24985</v>
       </c>
       <c r="E579">
         <v>0.58736</v>
       </c>
       <c r="F579">
-        <v>6.793817</v>
+        <v>6.798001</v>
       </c>
       <c r="G579">
         <v>0.669091</v>
@@ -25574,7 +25574,7 @@
         <v>0.994621</v>
       </c>
       <c r="N579">
-        <v>8.457529</v>
+        <v>8.461713</v>
       </c>
     </row>
     <row r="580" spans="1:14">
@@ -25585,16 +25585,16 @@
         <v>0.777225</v>
       </c>
       <c r="C580">
-        <v>2.874953</v>
+        <v>2.879873</v>
       </c>
       <c r="D580">
-        <v>2.061716</v>
+        <v>2.04956</v>
       </c>
       <c r="E580">
         <v>0.533937</v>
       </c>
       <c r="F580">
-        <v>6.247831</v>
+        <v>6.240595</v>
       </c>
       <c r="G580">
         <v>0.618623</v>
@@ -25612,13 +25612,57 @@
         <v>0.268881</v>
       </c>
       <c r="L580">
-        <v>0.330796</v>
+        <v>0.33023</v>
       </c>
       <c r="M580">
-        <v>0.919636</v>
+        <v>0.91907</v>
       </c>
       <c r="N580">
-        <v>7.786089</v>
+        <v>7.778287</v>
+      </c>
+    </row>
+    <row r="581" spans="1:14">
+      <c r="A581" s="6">
+        <v>43952</v>
+      </c>
+      <c r="B581">
+        <v>0.738349</v>
+      </c>
+      <c r="C581">
+        <v>2.813364</v>
+      </c>
+      <c r="D581">
+        <v>1.766636</v>
+      </c>
+      <c r="E581">
+        <v>0.530557</v>
+      </c>
+      <c r="F581">
+        <v>5.848906</v>
+      </c>
+      <c r="G581">
+        <v>0.672653</v>
+      </c>
+      <c r="H581">
+        <v>0.268273</v>
+      </c>
+      <c r="I581">
+        <v>0.017959</v>
+      </c>
+      <c r="J581">
+        <v>0.134061</v>
+      </c>
+      <c r="K581">
+        <v>0.256554</v>
+      </c>
+      <c r="L581">
+        <v>0.363949</v>
+      </c>
+      <c r="M581">
+        <v>1.040796</v>
+      </c>
+      <c r="N581">
+        <v>7.562355</v>
       </c>
     </row>
   </sheetData>
@@ -28877,13 +28921,13 @@
         <v>34.902356</v>
       </c>
       <c r="D83">
-        <v>25.440475</v>
+        <v>25.473071</v>
       </c>
       <c r="E83">
         <v>6.336608</v>
       </c>
       <c r="F83">
-        <v>80.947496</v>
+        <v>80.980092</v>
       </c>
       <c r="G83">
         <v>8.462374</v>
@@ -28907,7 +28951,7 @@
         <v>11.636976</v>
       </c>
       <c r="N83">
-        <v>101.046846</v>
+        <v>101.079442</v>
       </c>
     </row>
   </sheetData>

</xml_diff>